<commit_message>
added special exceptions for titanium_base
</commit_message>
<xml_diff>
--- a/data/abutments/abutments_unsh.xlsx
+++ b/data/abutments/abutments_unsh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L1ON\Documents\Работа\ОРТОС\Отчет по производству\data_13.04.2022\abutments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L1ON\Documents\Работа\ОРТОС\Отчет по производству\data_20.04.2022\abutments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D8C032-5597-476F-8654-A6FD8698AE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D671303-6046-4C25-B580-646EC14D8BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Отбор:</t>
   </si>
@@ -56,30 +56,42 @@
     <t>Абатмент временный</t>
   </si>
   <si>
+    <t>35792V2 Абатмент временный LM (собств. разр.) Straumann SynOcta RN (4.8) D=5 с позиционером без внутр. резьбы V.2</t>
+  </si>
+  <si>
+    <t>35973 Абатмент временный LM (собств. разр.) Osstem Implant Mini (3.5) D=4 с позиционером без внутр. резьбы V.1</t>
+  </si>
+  <si>
+    <t>35001уп Абатмент временный LM (собств. разр.) Ankylos X D=4.1 с позиционером без внутр. резьбы V.1 / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
     <t>35951 Абатмент временный LM (собств. разр.) Nobel Active RP (4.5), Nobel Conical Connection RP (4.3) D=4.4 с позиционером с внутр. резьбой V.1 / БЕЗ В</t>
   </si>
   <si>
-    <t>35792V2 Абатмент временный LM (собств. разр.) Straumann SynOcta RN (4.8) D=5 с позиционером без внутр. резьбы V.2</t>
-  </si>
-  <si>
-    <t>35001уп Абатмент временный LM (собств. разр.) Ankylos X D=4.1 с позиционером без внутр. резьбы V.1 / 1 ВИНТ, УПАК</t>
+    <t>35981 Абатмент временный LM (собств. разр.) Nobel Conical Connection NP (3.5) D=4.1 с позиционером без внутр. резьбы V.1</t>
+  </si>
+  <si>
+    <t>35001 Абатмент временный LM (собств. разр.) Ankylos X D=4.1 с позиционером без внутр. резьбы V.1 / БЕЗ ВИНТА</t>
   </si>
   <si>
     <t>35000уп Абатмент временный LM (собств. разр.) Implantium D=4.5 с позиционером без внутр. резьбы V.1 / 1 ВИНТ, В БЛИСТЕРЕ</t>
   </si>
   <si>
+    <t>35790 Абатмент временный LM (собств. разр.) Straumann Bone Level NC (3.3) D=4 с позиционером без внутр. резьбы V.1</t>
+  </si>
+  <si>
+    <t>35966 Абатмент временный LM (собств. разр.) Alpha Bio Internal D=4.5 с позиционером с внутр. резьбой V.1</t>
+  </si>
+  <si>
     <t>35000уп2 Абатмент временный LM (собств. разр.) Implantium D=4.5 с позиционером без внутр. резьбы V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
-    <t>35974опт Абатмент временный LM (собств. разр.) MegaGen AnyOne D=4.5 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
-  </si>
-  <si>
-    <t>35973опт Абатмент временный LM (собств. разр.) Osstem Implant Mini (3.5) D=4 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
-  </si>
-  <si>
     <t>35791 Абатмент временный LM (собств. разр.) Straumann Bone Level RC ( 4.1/4.8) D=4.4 с позиционером без внутр. резьбы V.1</t>
   </si>
   <si>
+    <t>35975опт Абатмент временный LM (собств. разр.) MegaGen AnyRidge D=4 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
+  </si>
+  <si>
     <t>35014 Абатмент временный LM (копия оригинала) Astra Tech 3.5/4.0 D=4.1 с позиционером без внутр. резьбы (арт. 24281) V.1 / БЕЗ ВИНТА</t>
   </si>
   <si>
@@ -89,51 +101,45 @@
     <t>35001уп2 Абатмент временный LM (собств. разр.) Ankylos X D=4.1 с позиционером без внутр. резьбы V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
-    <t>35930уп Абатмент временный LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 с позиционером без внутр. резьбы V.1 / 1 ВИНТ, В БЛИСТЕРЕ</t>
-  </si>
-  <si>
-    <t>35973уп2 Абатмент временный LM (собств. разр.) Osstem Implant Mini (3.5) D=4 с позиционером без внутр. резьбы V.1 / 2 ВИНТА, УПАК</t>
-  </si>
-  <si>
-    <t>35975 Абатмент временный LM (собств. разр.) MegaGen AnyRidge D=4 с позиционером без внутр. резьбы V.1</t>
+    <t>35965уп Абатмент временный LM (собств. разр.) Implantium D=4.5 с позиционером без внутр. резьбы V.1 / 1 ВИНТ, В БЛИСТЕРЕ</t>
+  </si>
+  <si>
+    <t>35967опт Абатмент временный LM (собств. разр.) Astra Tech 3.5/4.0 D=4.1 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
   </si>
   <si>
     <t>35002уп2 Абатмент временный LM (копия оригинала) Astra Tech 3.0 D=3.4 с позиционером без внутр. резьбы (арт. 25018) V.1 / 2 ВИНТА, В БЛИСТЕРЕ</t>
   </si>
   <si>
+    <t>35968опт Абатмент временный LM (собств. разр.) Astra Tech 4.5/5.0 D=4.5 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
+  </si>
+  <si>
     <t>35024 Абатмент временный LM (копия оригинала) Osstem Implant Mini (3.5) D=4 с позиционером без внутр. резьбы (арт. GSTTA4010TH) V.1 / БЕЗ ВИНТА</t>
   </si>
   <si>
-    <t>35975опт Абатмент временный LM (собств. разр.) MegaGen AnyRidge D=4 с позиционером без внутр. резьбы V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
-  </si>
-  <si>
     <t>Абатмент приливаемый</t>
   </si>
   <si>
-    <t>35214СБ Абатмент приливаемый LM (собств. разр.) MegaGen AnyRidge D=4.5 G/H=1.35 с позиционером V.1 / В СБОРЕ С КОЛПАЧКОМ</t>
-  </si>
-  <si>
     <t>35202СБуп2 Абатмент приливаемый LM (собств. разр.) Implantium D=4.5 G/H=1.25 с позиционером V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
+    <t>35797СБуп2 Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 без позиционера V.1 / 2 ВИНТА, УПАК</t>
+  </si>
+  <si>
+    <t>35200СБуп2 Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 с позиционером V.1 / 2 ВИНТА, УПАК</t>
+  </si>
+  <si>
     <t>35798СБуп2 Абатмент приливаемый LM (собств. разр.) Implantium D=4.5 G/H=1.25 без позиционера V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
-    <t>35797СБуп2 Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 без позиционера V.1 / 2 ВИНТА, УПАК</t>
+    <t>35797СБ Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 без позиционера V.1 / В СБОРЕ С КОЛПАЧКОМ</t>
+  </si>
+  <si>
+    <t>35796СБ Абатмент приливаемый LM (собств. разр.) Osstem Implant Mini (3.5) D=4.5 G/H=3.5 без позиционера V.1 / В СБОРЕ С КОЛПАЧКОМ</t>
   </si>
   <si>
     <t>35214СБуп2 Абатмент приливаемый LM (собств. разр.) MegaGen AnyRidge D=4.5 G/H=1.35 с позиционером V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
-    <t>35200СБуп2 Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 с позиционером V.1 / 2 ВИНТА, УПАК</t>
-  </si>
-  <si>
-    <t>35797СБ Абатмент приливаемый LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1.5 без позиционера V.1 / В СБОРЕ С КОЛПАЧКОМ</t>
-  </si>
-  <si>
-    <t>35796СБ Абатмент приливаемый LM (собств. разр.) Osstem Implant Mini (3.5) D=4.5 G/H=3.5 без позиционера V.1 / В СБОРЕ С КОЛПАЧКОМ</t>
-  </si>
-  <si>
     <t>35215СБуп2 Абатмент приливаемый LM (собств. разр.) Astra Tech 4.5/5.0 D=4.5 G/H=1.1 с позиционером V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
@@ -143,9 +149,30 @@
     <t>Абатмент прямой</t>
   </si>
   <si>
+    <t>36011 Абатмент прямой LM (копия оригинала) Adin RS (3.5/3.75/4.2/5.0/6.0) D=4.5 G/H=2 с позиционером с внутр. резьбой (арт. RS3802) V.1</t>
+  </si>
+  <si>
+    <t>36010 Абатмент прямой LM (копия оригинала) Adin RS (3.5/3.75/4.2/5.0/6.0) D=4.5 G/H=1 с позиционером с внутр. резьбой (арт. RS3801) V.1</t>
+  </si>
+  <si>
+    <t>35041 Абатмент прямой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1 с позиционером без внутр. резьбы (арт. GSTAS4611W) V.1 / Б</t>
+  </si>
+  <si>
     <t>35052уп2 Абатмент прямой LM (копия оригинала) Niko 3.5 D=4.5 G/H=2 с позиционером без внутр. резьбы (арт. 2.404) V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
+    <t>35080 Абатмент прямой LM (копия оригинала) Implantium D=5.5 G/H=3.5 с позиционером без внутр. резьбы (арт. DAB5535HL) V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
+    <t>36012 Абатмент прямой LM (копия оригинала) Adin RS (3.5/3.75/4.2/5.0/6.0) D=4.5 G/H=3 с позиционером с внутр. резьбой (арт. RS3803) V.1</t>
+  </si>
+  <si>
+    <t>35028 Абатмент прямой LM (копия оригинала) Implantium D=4.5 G/H=1 с позиционером без внутр. резьбы (арт. DAB4510HL) V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
+    <t>35076 Абатмент прямой LM (копия оригинала) Implantium D=4.5 G/H=2.5 с позиционером без внутр. резьбы (арт. DAB4525HL) V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
     <t>35016уп2 Абатмент прямой LM (копия оригинала) Alpha Bio Internal D=4.5 G/H=1.6 с позиционером с внутр. резьбой (арт. TLA5030) V.1 / 2 ВИНТА, УПАК</t>
   </si>
   <si>
@@ -161,19 +188,19 @@
     <t>35022уп2 Абатмент прямой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=5 G/H=2 H=5.5 с позиционером без внутр. резьбы (арт. GSTA5620WH)</t>
   </si>
   <si>
-    <t>35041 Абатмент прямой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1 с позиционером без внутр. резьбы (арт. GSTAS4611W) V.1 / Б</t>
+    <t>35019опт Абатмент прямой LM (копия оригинала) Alpha Bio Internal D=4.5 G/H=3 с позиционером с внутр. резьбой (арт. TLA3 5350) V.1 / ВКЛ. 1 ВИНТ, ИМ АБ</t>
   </si>
   <si>
     <t>35041П Абатмент прямой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=1 с позиционером без внутр. резьбы (арт. GSTAS4611W) ПОЛИР.</t>
   </si>
   <si>
-    <t>35078опт Абатмент прямой LM (копия оригинала) Implantium D=5.5 G/H=1.5 с позиционером без внутр. резьбы (арт. DAB5515HL) V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/О</t>
+    <t>35116опт Абатмент прямой LM (копия оригинала) Osstem Implant Mini (3.5) D=4.6 G/H=5 с позиционером без внутр. резьбы (арт. GSTA4651WH) V.1 / ВКЛ. 1 ВИ</t>
   </si>
   <si>
     <t>35004уп2 Абатмент прямой LM (копия оригинала) Osstem Implant Mini (3.5) D=4.5 G/H=2 с позиционером без внутр. резьбы (арт. GSTA4621WH) V.1 / 2 ВИНТА,</t>
   </si>
   <si>
-    <t>35116опт Абатмент прямой LM (копия оригинала) Osstem Implant Mini (3.5) D=4.6 G/H=5 с позиционером без внутр. резьбы (арт. GSTA4651WH) V.1 / ВКЛ. 1 ВИ</t>
+    <t>35154опт Абатмент прямой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=5 G/H=1 с позиционером без внутр. резьбы (арт. GSTA5610WH) V.1 /</t>
   </si>
   <si>
     <t>35007уп2 Абатмент прямой LM (копия оригинала) Dentis Regular D=4.5 G/H=2 с позиционером без внутр. резьбы (арт. DSSA4520PCTS) V.1 / 2 ВИНТА, УПАК</t>
@@ -182,94 +209,106 @@
     <t>Абатмент прямой Multi-unit</t>
   </si>
   <si>
+    <t>36092 Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=2 V.1</t>
+  </si>
+  <si>
+    <t>36093 Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=3 V.1</t>
+  </si>
+  <si>
+    <t>36093опт Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=3 V.1 / ВКЛ. МАНЖЕТУ, ИМ АБ.</t>
+  </si>
+  <si>
+    <t>35576Пуп Абатмент прямой MU LM (копия оригинала) MegaGen AnyOne Multi-Unit Type S D=5 G/H=2.5 (арт. MU5025HT) ПОЛИР. V.1.P / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
+    <t>35575Пуп Абатмент прямой MU LM (копия оригинала) MegaGen AnyOne Multi-Unit Type S D=5 G/H=1.5 (арт. MU5015HT) ПОЛИР. V.1.P / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
     <t>36091 Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=1 V.1</t>
   </si>
   <si>
-    <t>35576Пуп Абатмент прямой MU LM (копия оригинала) MegaGen AnyOne Multi-Unit Type S D=5 G/H=2.5 (арт. MU5025HT) ПОЛИР. V.1.P / 1 ВИНТ, УПАК</t>
-  </si>
-  <si>
-    <t>36092 Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=2 V.1</t>
-  </si>
-  <si>
-    <t>36093 Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=3 V.1</t>
-  </si>
-  <si>
-    <t>35575Пуп Абатмент прямой MU LM (копия оригинала) MegaGen AnyOne Multi-Unit Type S D=5 G/H=1.5 (арт. MU5015HT) ПОЛИР. V.1.P / 1 ВИНТ, УПАК</t>
-  </si>
-  <si>
     <t>36088 Абатмент прямой MU LM (собств. разр.) Osstem Implant Mini (3.5) D=4.8 G/H=1 V.1</t>
   </si>
   <si>
-    <t>36091опт Абатмент прямой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0), Implantium, MegaGen AnyOne D=4.8 G/H=1 V.1 / ВКЛ. МАНЖЕТУ, ИМ АБ.</t>
-  </si>
-  <si>
-    <t>36090 Абатмент прямой MU LM (собств. разр.) Osstem Implant Mini (3.5) D=4.8 G/H=3 V.1</t>
-  </si>
-  <si>
-    <t>36089 Абатмент прямой MU LM (собств. разр.) Osstem Implant Mini (3.5) D=4.8 G/H=2 V.1</t>
-  </si>
-  <si>
     <t>Абатмент угловой</t>
   </si>
   <si>
+    <t>35816 Абатмент угловой LM (копия оригинала) Implantium D=5.6 G/H=1.75 Угол=15 с позиционером без внутр. резьбы (арт. AAB155520HL) V.1</t>
+  </si>
+  <si>
+    <t>35801 Абатмент угловой LM (копия оригинала) Implantium D=4.5 G/H=2 Угол=15 с позиционером без внутр. резьбы (арт. AAB154520HL) V.1</t>
+  </si>
+  <si>
     <t>35046уп2 Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=2 Угол=17 с позиционером без внутр. резьбы (арт. GSAA452</t>
   </si>
   <si>
-    <t>35828Попт Абатмент угловой LM (копия оригинала) MegaGen AnyOne D=4.5 G/H=4.5 Угол=15 с позиционером без внутр. резьбы (арт. AA4415HT) ПОЛИР. V.1.P / В</t>
+    <t>35045опт Абатмент угловой LM (копия оригинала) Osstem Implant Mini (3.5) D=4.5 G/H=2 Угол=17 с позиционером без внутр. резьбы (арт. GSAA4520MAWH) V.1</t>
+  </si>
+  <si>
+    <t>35047опт Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=4 Угол=17 с позиционером без внутр. резьбы (арт. GSAA454</t>
+  </si>
+  <si>
+    <t>35046опт Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=2 Угол=17 с позиционером без внутр. резьбы (арт. GSAA452</t>
   </si>
   <si>
     <t>я НЕ ИСП !!!350461уп2 Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=2 Угол=17 с позиционером без внутр. резьбы</t>
   </si>
   <si>
-    <t>35829опт Абатмент угловой LM (копия оригинала) MegaGen AnyOne D=5.5 G/H=2.5 Угол=15 с позиционером без внутр. резьбы (арт. AA5215HT) V.1 / ВКЛ. 1 ВИНТ</t>
-  </si>
-  <si>
-    <t>35047опт Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=4 Угол=17 с позиционером без внутр. резьбы (арт. GSAA454</t>
-  </si>
-  <si>
-    <t>35046опт Абатмент угловой LM (копия оригинала) Osstem Implant Regular (4.0/4.5/5.0) D=4.5 G/H=2 Угол=17 с позиционером без внутр. резьбы (арт. GSAA452</t>
-  </si>
-  <si>
     <t>Абатмент угловой Multi-unit</t>
   </si>
   <si>
+    <t>36086уп Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
     <t>36094уп Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=2.5 Угол=17гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
-    <t>36086уп Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
-  </si>
-  <si>
     <t>35383уп Абатмент угловой MU LM (собств. разр.) Nobel Active RP (4.5) D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
     <t>36095уп Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=17гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
+    <t>36096уп Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
+    <t>35384уп Абатмент угловой MU LM (собств. разр.) Nobel Active RP (4.5) D=4.8 G/H=4.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
     <t>36097уп Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=4.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
-    <t>35384уп Абатмент угловой MU LM (собств. разр.) Nobel Active RP (4.5) D=4.8 G/H=4.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
-  </si>
-  <si>
-    <t>36096уп Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
-  </si>
-  <si>
     <t>36083уп Абатмент угловой MU LM (собств. разр.) Osstem Implant Mini (3.5) D=4.8 G/H=4.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
     <t>36084уп Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=2.5 Угол=17гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
   </si>
   <si>
-    <t>36086 Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / БЕЗ ВИНТА</t>
+    <t>44009уп Абатмент угловой MU LM (собств. разр.) MegaGen AnyOne D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / 1 ВИНТ, УПАК</t>
+  </si>
+  <si>
+    <t>44010 Абатмент угловой MU LM (собств. разр.) MegaGen AnyOne D=4.8 G/H=4.5 Угол=30гр. с позиционером V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
+    <t>44007 Абатмент угловой MU LM (собств. разр.) MegaGen AnyOne D=4.8 G/H=2.5 Угол=17гр. с позиционером V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
+    <t>44008 Абатмент угловой MU LM (собств. разр.) MegaGen AnyOne D=4.8 G/H=3.5 Угол=17гр. с позиционером V.1 / БЕЗ ВИНТА</t>
   </si>
   <si>
     <t>36094 Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=2.5 Угол=17гр. с позиционером V.1 / БЕЗ ВИНТА</t>
   </si>
   <si>
+    <t>36085опт Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=3.5 Угол=17гр. с позиционером V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.</t>
+  </si>
+  <si>
+    <t>36086опт Абатмент угловой MU LM (собств. разр.) Osstem Implant Regular (4.0/4.5/5.0) D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.</t>
+  </si>
+  <si>
+    <t>36096 Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / БЕЗ ВИНТА</t>
+  </si>
+  <si>
     <t>36095 Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=17гр. с позиционером V.1 / БЕЗ ВИНТА</t>
-  </si>
-  <si>
-    <t>36096опт Абатмент угловой MU LM (собств. разр.) Implantium D=4.8 G/H=3.5 Угол=30гр. с позиционером V.1 / ВКЛ. 1 ВИНТ, ИМ АБ.РУ/ОПТ</t>
   </si>
 </sst>
 </file>
@@ -348,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -372,9 +411,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -752,11 +788,9 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -767,8 +801,7 @@
     <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -776,41 +809,41 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
@@ -822,67 +855,65 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16">
-        <v>1535</v>
-      </c>
-      <c r="E6" s="16"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15">
+        <v>1430</v>
+      </c>
+      <c r="E6" s="15"/>
       <c r="F6" s="4">
-        <v>820</v>
+        <v>945</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="4">
-        <v>715</v>
+        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18">
-        <v>410</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="6">
-        <v>10</v>
-      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17">
+        <v>168</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6">
-        <v>400</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18">
-        <v>168</v>
-      </c>
-      <c r="E8" s="18"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17">
+        <v>50</v>
+      </c>
+      <c r="E8" s="17"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="6">
-        <v>168</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17">
         <v>40</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="6">
@@ -890,697 +921,705 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18">
-        <v>30</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="7"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17">
+        <v>40</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="6">
+        <v>10</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="6">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18">
-        <v>25</v>
-      </c>
-      <c r="E11" s="18"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17">
+        <v>130</v>
+      </c>
+      <c r="E11" s="17"/>
       <c r="F11" s="6">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18">
-        <v>15</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17">
+        <v>55</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="6">
+        <v>25</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="6">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18">
-        <v>10</v>
-      </c>
-      <c r="E13" s="18"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
+        <v>30</v>
+      </c>
+      <c r="E13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="6">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18">
-        <v>10</v>
-      </c>
-      <c r="E14" s="18"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17">
+        <v>20</v>
+      </c>
+      <c r="E14" s="17"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18">
-        <v>262</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="6">
-        <v>255</v>
-      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17">
+        <v>20</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="6">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18">
-        <v>452</v>
-      </c>
-      <c r="E16" s="18"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17">
+        <v>25</v>
+      </c>
+      <c r="E16" s="17"/>
       <c r="F16" s="6">
-        <v>445</v>
+        <v>10</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="6">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18">
-        <v>5</v>
-      </c>
-      <c r="E17" s="18"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17">
+        <v>14</v>
+      </c>
+      <c r="E17" s="17"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="6">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18">
-        <v>2</v>
-      </c>
-      <c r="E18" s="18"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17">
+        <v>10</v>
+      </c>
+      <c r="E18" s="17"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="6">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18">
-        <v>2</v>
-      </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17">
+        <v>262</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="6">
+        <v>255</v>
+      </c>
       <c r="G19" s="7"/>
       <c r="H19" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18">
-        <v>1</v>
-      </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17">
+        <v>452</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="6">
+        <v>445</v>
+      </c>
       <c r="G20" s="7"/>
       <c r="H20" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17">
+        <v>5</v>
+      </c>
+      <c r="E21" s="17"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18">
-        <v>101</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="6">
-        <v>100</v>
-      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17">
+        <v>4</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18">
-        <v>1</v>
-      </c>
-      <c r="E23" s="18"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17">
+        <v>2</v>
+      </c>
+      <c r="E23" s="17"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="19">
-        <v>787</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="4">
-        <v>43</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="4">
-        <v>744</v>
+      <c r="E24" s="17"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18">
-        <v>240</v>
-      </c>
-      <c r="E25" s="18"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="6">
-        <v>240</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18">
-        <v>220</v>
-      </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17">
+        <v>101</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="6">
+        <v>100</v>
+      </c>
       <c r="G26" s="7"/>
       <c r="H26" s="6">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="18">
-        <v>100</v>
+        <v>337</v>
       </c>
       <c r="E27" s="18"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="6">
-        <v>100</v>
+      <c r="F27" s="4">
+        <v>43</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="4">
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18">
-        <v>90</v>
-      </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="6">
-        <v>10</v>
-      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17">
+        <v>120</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="6">
-        <v>80</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="18">
-        <v>65</v>
-      </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="7"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17">
+        <v>90</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="6">
+        <v>10</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="6">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18">
-        <v>50</v>
-      </c>
-      <c r="E30" s="18"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17">
+        <v>70</v>
+      </c>
+      <c r="E30" s="17"/>
       <c r="F30" s="6">
         <v>30</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="6">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18">
-        <v>11</v>
-      </c>
-      <c r="E31" s="18"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17">
+        <v>30</v>
+      </c>
+      <c r="E31" s="17"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18">
-        <v>5</v>
-      </c>
-      <c r="E32" s="18"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18">
-        <v>2</v>
-      </c>
-      <c r="E33" s="18"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18">
-        <v>4</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="6">
-        <v>3</v>
-      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17">
+        <v>5</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="19">
-        <v>194</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="4">
-        <v>97</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="4">
-        <v>97</v>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17">
+        <v>2</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18">
-        <v>100</v>
-      </c>
-      <c r="E36" s="18"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17">
+        <v>4</v>
+      </c>
+      <c r="E36" s="17"/>
       <c r="F36" s="6">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="18">
-        <v>20</v>
+        <v>450</v>
       </c>
       <c r="E37" s="18"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="6">
-        <v>20</v>
+      <c r="F37" s="4">
+        <v>140</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="4">
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18">
-        <v>10</v>
-      </c>
-      <c r="E38" s="18"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17">
+        <v>50</v>
+      </c>
+      <c r="E38" s="17"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
       <c r="H38" s="6">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18">
-        <v>7</v>
-      </c>
-      <c r="E39" s="18"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17">
+        <v>50</v>
+      </c>
+      <c r="E39" s="17"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="6">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18">
-        <v>13</v>
-      </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="6">
-        <v>8</v>
-      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17">
+        <v>35</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="7"/>
       <c r="H40" s="6">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="18">
-        <v>22</v>
-      </c>
-      <c r="E41" s="18"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17">
+        <v>100</v>
+      </c>
+      <c r="E41" s="17"/>
       <c r="F41" s="6">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="6">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18">
-        <v>5</v>
-      </c>
-      <c r="E42" s="18"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17">
+        <v>20</v>
+      </c>
+      <c r="E42" s="17"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
       <c r="H42" s="6">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18">
-        <v>4</v>
-      </c>
-      <c r="E43" s="18"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="17">
+        <v>20</v>
+      </c>
+      <c r="E43" s="17"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="6">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18">
-        <v>3</v>
-      </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="17">
+        <v>33</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="6">
+        <v>13</v>
+      </c>
       <c r="G44" s="7"/>
       <c r="H44" s="6">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18">
-        <v>7</v>
-      </c>
-      <c r="E45" s="18"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="17">
+        <v>50</v>
+      </c>
+      <c r="E45" s="17"/>
       <c r="F45" s="6">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="18">
-        <v>2</v>
-      </c>
-      <c r="E46" s="18"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="17">
+        <v>20</v>
+      </c>
+      <c r="E46" s="17"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="18">
-        <v>1</v>
-      </c>
-      <c r="E47" s="18"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="17">
+        <v>10</v>
+      </c>
+      <c r="E47" s="17"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
       <c r="H47" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="19">
-        <v>31</v>
-      </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="4">
-        <v>31</v>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="17">
+        <v>7</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="18">
-        <v>10</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="7"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="17">
+        <v>13</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="6">
+        <v>8</v>
+      </c>
       <c r="G49" s="7"/>
       <c r="H49" s="6">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18">
-        <v>6</v>
-      </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="7"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="17">
+        <v>22</v>
+      </c>
+      <c r="E50" s="17"/>
+      <c r="F50" s="6">
+        <v>17</v>
+      </c>
       <c r="G50" s="7"/>
       <c r="H50" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18">
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="17">
         <v>4</v>
       </c>
-      <c r="E51" s="18"/>
+      <c r="E51" s="17"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="6">
@@ -1588,31 +1627,31 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="18">
-        <v>3</v>
-      </c>
-      <c r="E52" s="18"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="17">
+        <v>4</v>
+      </c>
+      <c r="E52" s="17"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18">
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="17">
         <v>2</v>
       </c>
-      <c r="E53" s="18"/>
+      <c r="E53" s="17"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
       <c r="H53" s="6">
@@ -1620,31 +1659,33 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18">
-        <v>2</v>
-      </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="7"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="17">
+        <v>7</v>
+      </c>
+      <c r="E54" s="17"/>
+      <c r="F54" s="6">
+        <v>5</v>
+      </c>
       <c r="G54" s="7"/>
       <c r="H54" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="18">
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17">
         <v>2</v>
       </c>
-      <c r="E55" s="18"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="6">
@@ -1652,115 +1693,111 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="18">
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="17">
         <v>1</v>
       </c>
-      <c r="E56" s="18"/>
+      <c r="E56" s="17"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
+    <row r="57" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="18">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="E57" s="18"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="19">
-        <v>18</v>
-      </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="4">
-        <v>2</v>
-      </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="4">
-        <v>16</v>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="17">
+        <v>14</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="6">
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="18">
-        <v>10</v>
-      </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="6">
-        <v>2</v>
-      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="17">
+        <v>13</v>
+      </c>
+      <c r="E59" s="17"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="6">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="18">
-        <v>2</v>
-      </c>
-      <c r="E60" s="18"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="17">
+        <v>7</v>
+      </c>
+      <c r="E60" s="17"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="18">
-        <v>2</v>
-      </c>
-      <c r="E61" s="18"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17">
+        <v>6</v>
+      </c>
+      <c r="E61" s="17"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="18">
-        <v>2</v>
-      </c>
-      <c r="E62" s="18"/>
+      <c r="E62" s="17"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="6">
@@ -1768,31 +1805,31 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="18">
-        <v>1</v>
-      </c>
-      <c r="E63" s="18"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17">
+        <v>2</v>
+      </c>
+      <c r="E63" s="17"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="18">
-        <v>1</v>
-      </c>
-      <c r="E64" s="18"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="6">
@@ -1800,253 +1837,493 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="19">
-        <v>245</v>
-      </c>
-      <c r="E65" s="19"/>
-      <c r="F65" s="5"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="18">
+        <v>70</v>
+      </c>
+      <c r="E65" s="18"/>
+      <c r="F65" s="4">
+        <v>4</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="4">
-        <v>245</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="18">
-        <v>30</v>
-      </c>
-      <c r="E66" s="18"/>
-      <c r="F66" s="7"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17">
+        <v>22</v>
+      </c>
+      <c r="E66" s="17"/>
+      <c r="F66" s="6">
+        <v>2</v>
+      </c>
       <c r="G66" s="7"/>
       <c r="H66" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="18">
-        <v>30</v>
-      </c>
-      <c r="E67" s="18"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="17">
+        <v>20</v>
+      </c>
+      <c r="E67" s="17"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
       <c r="H67" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="18">
-        <v>30</v>
-      </c>
-      <c r="E68" s="18"/>
-      <c r="F68" s="7"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="17">
+        <v>10</v>
+      </c>
+      <c r="E68" s="17"/>
+      <c r="F68" s="6">
+        <v>2</v>
+      </c>
       <c r="G68" s="7"/>
       <c r="H68" s="6">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="18">
-        <v>30</v>
-      </c>
-      <c r="E69" s="18"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="17">
+        <v>7</v>
+      </c>
+      <c r="E69" s="17"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
       <c r="H69" s="6">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="18">
-        <v>30</v>
-      </c>
-      <c r="E70" s="18"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="17">
+        <v>5</v>
+      </c>
+      <c r="E70" s="17"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
       <c r="H70" s="6">
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="18">
-        <v>30</v>
-      </c>
-      <c r="E71" s="18"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="17">
+        <v>4</v>
+      </c>
+      <c r="E71" s="17"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
       <c r="H71" s="6">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="18">
-        <v>30</v>
-      </c>
-      <c r="E72" s="18"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="17">
+        <v>2</v>
+      </c>
+      <c r="E72" s="17"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
       <c r="H72" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="18">
-        <v>15</v>
+        <v>302</v>
       </c>
       <c r="E73" s="18"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="6">
-        <v>15</v>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="4">
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="18">
-        <v>13</v>
-      </c>
-      <c r="E74" s="18"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="17">
+        <v>34</v>
+      </c>
+      <c r="E74" s="17"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
       <c r="H74" s="6">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="18">
-        <v>3</v>
-      </c>
-      <c r="E75" s="18"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="17">
+        <v>30</v>
+      </c>
+      <c r="E75" s="17"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
       <c r="H75" s="6">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18">
-        <v>2</v>
-      </c>
-      <c r="E76" s="18"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="17">
+        <v>30</v>
+      </c>
+      <c r="E76" s="17"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
       <c r="H76" s="6">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="18">
-        <v>1</v>
-      </c>
-      <c r="E77" s="18"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="17">
+        <v>30</v>
+      </c>
+      <c r="E77" s="17"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
       <c r="H77" s="6">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="18">
-        <v>1</v>
-      </c>
-      <c r="E78" s="18"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="17">
+        <v>30</v>
+      </c>
+      <c r="E78" s="17"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="17">
+        <v>30</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="17">
+        <v>30</v>
+      </c>
+      <c r="E80" s="17"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="17">
+        <v>15</v>
+      </c>
+      <c r="E81" s="17"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="17">
+        <v>15</v>
+      </c>
+      <c r="E82" s="17"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="17">
+        <v>12</v>
+      </c>
+      <c r="E83" s="17"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="17">
+        <v>12</v>
+      </c>
+      <c r="E84" s="17"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="17">
+        <v>12</v>
+      </c>
+      <c r="E85" s="17"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="17">
+        <v>12</v>
+      </c>
+      <c r="E86" s="17"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="17">
+        <v>5</v>
+      </c>
+      <c r="E87" s="17"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="17">
+        <v>2</v>
+      </c>
+      <c r="E88" s="17"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="14" t="s">
+      <c r="E89" s="17"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="17">
+        <v>1</v>
+      </c>
+      <c r="E90" s="17"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="21.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="17">
+        <v>1</v>
+      </c>
+      <c r="E91" s="17"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B79" s="14"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="20">
-        <v>2810</v>
-      </c>
-      <c r="E79" s="20"/>
-      <c r="F79" s="9">
-        <v>962</v>
-      </c>
-      <c r="G79" s="10"/>
-      <c r="H79" s="8">
-        <v>1848</v>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="19">
+        <v>2634</v>
+      </c>
+      <c r="E92" s="19"/>
+      <c r="F92" s="8">
+        <v>1132</v>
+      </c>
+      <c r="G92" s="9"/>
+      <c r="H92" s="8">
+        <v>1502</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="153">
+  <mergeCells count="179">
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="A83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A87:C87"/>
+    <mergeCell ref="D87:E87"/>
     <mergeCell ref="A78:C78"/>
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="D79:E79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="D82:E82"/>
     <mergeCell ref="A73:C73"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="A74:C74"/>

</xml_diff>